<commit_message>
ADD MAN HINH QUAN LI DAO TAO
</commit_message>
<xml_diff>
--- a/danhsachdiemsinhvien.xlsx
+++ b/danhsachdiemsinhvien.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\lap trinh\C++Project\MFC_QLDSV\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\lap trinh\C++Project\MFC_QuanLyDiemSinhVien\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11460" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11460"/>
   </bookViews>
   <sheets>
     <sheet name="KETQUA" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="1" hidden="1">Sheet2!$A$1:$F$5</definedName>
+    <definedName name="ExternalData_1" localSheetId="1" hidden="1">Sheet2!$A$1:$F$3</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
   <si>
     <t>MSSV</t>
   </si>
@@ -195,8 +195,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="KETQUA_2" displayName="KETQUA_2" ref="A1:F5" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:F5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="KETQUA_2" displayName="KETQUA_2" ref="A1:F3" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:F3"/>
   <tableColumns count="6">
     <tableColumn id="13" uniqueName="13" name="MSSV" queryTableFieldId="1" dataDxfId="5"/>
     <tableColumn id="14" uniqueName="14" name="MALOP" queryTableFieldId="2" dataDxfId="4"/>
@@ -474,8 +474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="A1:F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -587,10 +587,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -627,13 +627,13 @@
         <v>4201198001</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D2" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E2" s="1">
         <v>9</v>
@@ -642,57 +642,21 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" s="1">
-        <v>4201198001</v>
+        <v>4201108981</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1">
+        <v>6</v>
+      </c>
+      <c r="D3" s="1">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1">
         <v>7</v>
       </c>
-      <c r="C3" s="1">
-        <v>5</v>
-      </c>
-      <c r="D3" s="1">
-        <v>8</v>
-      </c>
-      <c r="E3" s="1">
-        <v>8</v>
-      </c>
       <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A4" s="1">
-        <v>4201198001</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="1">
-        <v>7</v>
-      </c>
-      <c r="D4" s="1">
-        <v>8</v>
-      </c>
-      <c r="E4" s="1">
-        <v>9</v>
-      </c>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A5" s="1">
-        <v>4201108981</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="1">
-        <v>6</v>
-      </c>
-      <c r="D5" s="1">
-        <v>8</v>
-      </c>
-      <c r="E5" s="1">
-        <v>7</v>
-      </c>
-      <c r="F5" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>